<commit_message>
Made Changes in Test
</commit_message>
<xml_diff>
--- a/Output-ss/ExcelFIles/OutputXLFile.xlsx
+++ b/Output-ss/ExcelFIles/OutputXLFile.xlsx
@@ -6,14 +6,14 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="carWashServices" r:id="rId5" sheetId="7"/>
     <sheet name="GymNames" r:id="rId4" sheetId="8"/>
+    <sheet name="carWashServices" r:id="rId5" sheetId="9"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="72">
   <si>
     <t>CarWashServiceName</t>
   </si>
@@ -271,67 +271,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>62</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>64</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>66</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>68</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>69</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:A31"/>
@@ -498,4 +437,65 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>